<commit_message>
More weak encryption for spreadsheet data
</commit_message>
<xml_diff>
--- a/Basketball Stats.xlsx
+++ b/Basketball Stats.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t>Opponent</t>
   </si>
@@ -40,7 +40,7 @@
     <t>~50</t>
   </si>
   <si>
-    <t>Winchester 8GB</t>
+    <t>Wuxqykdwks</t>
   </si>
   <si>
     <t>First Name</t>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>Cambridge 8A</t>
   </si>
   <si>
     <t xml:space="preserve">vs. Sehmesi 12/02/2018 12:30 pm
@@ -2057,7 +2054,7 @@
     </row>
     <row r="25">
       <c r="A25" s="36" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -2305,15 +2302,15 @@
     </row>
     <row r="31">
       <c r="A31" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="U31" s="49" t="s">
         <v>64</v>
-      </c>
-      <c r="U31" s="49" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="32">
       <c r="U32" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91">

</xml_diff>